<commit_message>
Add height in meters to network sites
</commit_message>
<xml_diff>
--- a/templates/Network Sites.xlsx
+++ b/templates/Network Sites.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -33,8 +33,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>A descriptive name for the site. This will be displayed in Sonar.</t>
+          <t xml:space="preserve">A descriptive name for the site. This will be displayed in Sonar.</t>
         </r>
       </text>
     </comment>
@@ -45,8 +46,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Either the address or the latitude and longitude is required. If you only provide the address, you must enable address verification so that Sonar can try to calculate the latitude and longitude. Including the latitude and longitude is strongly recommended, otherwise it is likely you will receive some failures.</t>
+          <t xml:space="preserve">Either the address or the latitude and longitude is required. If you only provide the address, you must enable address verification so that Sonar can try to calculate the latitude and longitude. Including the latitude and longitude is strongly recommended, otherwise it is likely you will receive some failures.</t>
         </r>
       </text>
     </comment>
@@ -57,8 +59,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>Must a valid state for the country. You can get a list of states from the Sonar API endpoint /_data/subdivisions/:country</t>
+          <t xml:space="preserve">Must a valid state for the country. You can get a list of states from the Sonar API endpoint /_data/subdivisions/:country</t>
         </r>
       </text>
     </comment>
@@ -69,8 +72,9 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>This must be a two character country code (e.g. US)</t>
+          <t xml:space="preserve">This must be a two character country code (e.g. US)</t>
         </r>
       </text>
     </comment>
@@ -81,8 +85,22 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
-          <t>You must include either the address (and enable address verification in the importer) or the latitude and longitude. It is strongly recommended that you include the latitude and longitude, especially if your network site is not on a main street.</t>
+          <t xml:space="preserve">You must include either the address (and enable address verification in the importer) or the latitude and longitude. It is strongly recommended that you include the latitude and longitude, especially if your network site is not on a main street.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">The height of the structure, in meters.</t>
         </r>
       </text>
     </comment>
@@ -91,33 +109,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Address Line 1</t>
-  </si>
-  <si>
-    <t>Address Line 2</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>ZIP</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Line 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address Line 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZIP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Height in Meters</t>
   </si>
 </sst>
 </file>
@@ -125,13 +146,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -151,13 +173,14 @@
     <font>
       <sz val="12"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -310,19 +333,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>782640</xdr:colOff>
+      <xdr:colOff>782280</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="30240" y="9720"/>
-          <a:ext cx="8067600" cy="6148440"/>
+          <a:ext cx="7952760" cy="6148080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -334,28 +357,80 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>Use this sheet to import network sites into Sonar. The address provided should be the physical address the site is located at. You can provide a country, latitude and longitude without an address – the most important data is the latitude and longitude to get proper placement on the map. If you don't know the latitude and longitude, you can exclude it and enable address verification in the importer for the network site to try to calculate it.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>Grey columns are required, blue columns are optional.</a:t>
           </a:r>
-          <a:endParaRPr/>
+          <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -377,7 +452,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -399,13 +474,15 @@
   <dimension ref="1:1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="17.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="17.4132653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="18.9234693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -436,12 +513,15 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>